<commit_message>
Potentially solved part 2 of day 6
Copying the entire grid object so I can add a potential obstacle and check if hitting this obstacle would put the guard in a loop
</commit_message>
<xml_diff>
--- a/adventofcode/2024/6/griddy.xlsx
+++ b/adventofcode/2024/6/griddy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\johnginnane.github.io\adventofcode\2024\6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1174A2E-E651-4583-A237-0F709C240220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35A50BF-773F-421E-9853-24A658B63807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15630" yWindow="3345" windowWidth="13740" windowHeight="14370" xr2:uid="{9ACED5B0-2B8F-49AE-9824-F2A59173B6AB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="13">
   <si>
     <t>^</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>7,6</t>
+  </si>
+  <si>
+    <t>3,8</t>
+  </si>
+  <si>
+    <t>1,8</t>
+  </si>
+  <si>
+    <t>7,7</t>
+  </si>
+  <si>
+    <t>7,9</t>
   </si>
 </sst>
 </file>
@@ -539,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65D9E-6C2D-41D9-A72C-7B476B848810}">
-  <dimension ref="B2:W22"/>
+  <dimension ref="B1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,6 +568,38 @@
     <col min="1" max="16384" width="3.28515625" style="3"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="N1" s="3">
+        <v>0</v>
+      </c>
+      <c r="O1" s="3">
+        <v>1</v>
+      </c>
+      <c r="P1" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>3</v>
+      </c>
+      <c r="R1" s="3">
+        <v>4</v>
+      </c>
+      <c r="S1" s="3">
+        <v>5</v>
+      </c>
+      <c r="T1" s="3">
+        <v>6</v>
+      </c>
+      <c r="U1" s="3">
+        <v>7</v>
+      </c>
+      <c r="V1" s="3">
+        <v>8</v>
+      </c>
+      <c r="W1" s="3">
+        <v>9</v>
+      </c>
+    </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -561,6 +611,9 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -593,6 +646,9 @@
         <v>2</v>
       </c>
       <c r="K3" s="2"/>
+      <c r="M3" s="3">
+        <v>1</v>
+      </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -623,6 +679,9 @@
         <v>1</v>
       </c>
       <c r="K4" s="1"/>
+      <c r="M4" s="3">
+        <v>2</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -649,6 +708,9 @@
         <v>1</v>
       </c>
       <c r="K5" s="1"/>
+      <c r="M5" s="3">
+        <v>3</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="6"/>
@@ -685,6 +747,9 @@
         <v>1</v>
       </c>
       <c r="K6" s="1"/>
+      <c r="M6" s="3">
+        <v>4</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -717,6 +782,9 @@
         <v>1</v>
       </c>
       <c r="K7" s="1"/>
+      <c r="M7" s="3">
+        <v>5</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -753,6 +821,9 @@
         <v>2</v>
       </c>
       <c r="K8" s="1"/>
+      <c r="M8" s="3">
+        <v>6</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="6"/>
       <c r="P8" s="1"/>
@@ -795,6 +866,9 @@
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="1"/>
+      <c r="M9" s="3">
+        <v>7</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -835,6 +909,9 @@
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
+      <c r="M10" s="3">
+        <v>8</v>
+      </c>
       <c r="N10" s="6"/>
       <c r="O10" s="9">
         <v>8</v>
@@ -862,6 +939,9 @@
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
+      <c r="M11" s="3">
+        <v>9</v>
+      </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -876,10 +956,10 @@
       <c r="W11" s="1"/>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="N13" s="3">
-        <v>1</v>
-      </c>
-      <c r="O13" s="8" t="s">
+      <c r="O13" s="3">
+        <v>1</v>
+      </c>
+      <c r="P13" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -888,10 +968,10 @@
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
-      <c r="N14" s="3">
-        <v>2</v>
-      </c>
-      <c r="O14" s="8" t="s">
+      <c r="O14" s="3">
+        <v>2</v>
+      </c>
+      <c r="P14" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -900,10 +980,10 @@
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
-      <c r="N15" s="3">
-        <v>3</v>
-      </c>
-      <c r="O15" s="8" t="s">
+      <c r="O15" s="3">
+        <v>3</v>
+      </c>
+      <c r="P15" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -912,62 +992,80 @@
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
-      <c r="N16" s="3">
+      <c r="O16" s="3">
         <v>4</v>
       </c>
-      <c r="O16" s="8" t="s">
+      <c r="P16" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
-      <c r="N17" s="3">
+      <c r="N17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O17" s="3">
         <v>5</v>
       </c>
-      <c r="O17" s="8" t="s">
+      <c r="P17" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="N18" s="3">
+    <row r="18" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O18" s="3">
         <v>6</v>
       </c>
-      <c r="O18" s="8" t="s">
+      <c r="P18" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="N19" s="3">
+    <row r="19" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O19" s="3">
         <v>7</v>
       </c>
-      <c r="O19" s="8" t="s">
+      <c r="P19" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="N20" s="3">
+    <row r="20" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O20" s="3">
         <v>8</v>
       </c>
-      <c r="O20" s="8" t="s">
+      <c r="P20" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="N21" s="3">
+    <row r="21" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O21" s="3">
         <v>9</v>
       </c>
-      <c r="O21" s="8" t="s">
+      <c r="P21" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="N22" s="3">
+    <row r="22" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22" s="3">
         <v>10</v>
       </c>
-      <c r="O22" s="8" t="s">
+      <c r="P22" s="8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>